<commit_message>
Updated distance based scoring to enable gradual decay of scoring.
</commit_message>
<xml_diff>
--- a/checklist/Residential Building.xlsx
+++ b/checklist/Residential Building.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Liveable Cities Score\checklist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F468818-B306-428F-952E-DFA2FC6733B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D8C3D48-1E07-4726-AB73-BDEA99364E33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19695" yWindow="0" windowWidth="18630" windowHeight="16200" xr2:uid="{ECB84FC6-903A-43DA-9768-BC3FCD298BC1}"/>
+    <workbookView xWindow="19665" yWindow="0" windowWidth="18735" windowHeight="16200" xr2:uid="{ECB84FC6-903A-43DA-9768-BC3FCD298BC1}"/>
   </bookViews>
   <sheets>
     <sheet name="LCS" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="54">
   <si>
     <t>Feature is present</t>
   </si>
@@ -84,9 +84,6 @@
     <t>+ Sidewalk is at least 2m wide</t>
   </si>
   <si>
-    <t>Street access to dedicated bicycle lane (at least 1.5m wide)</t>
-  </si>
-  <si>
     <t>Base Score</t>
   </si>
   <si>
@@ -217,6 +214,12 @@
   </si>
   <si>
     <t>+ Sidewalk is protected by street parking. Item is checked if no vehicle traffic is allowed.</t>
+  </si>
+  <si>
+    <t>absent</t>
+  </si>
+  <si>
+    <t>Street access to dedicated bicycle lane (at least 1.5m wide; at most 20m from building entrance)</t>
   </si>
 </sst>
 </file>
@@ -325,7 +328,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -337,10 +340,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="3" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -354,6 +353,9 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="9" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Accent1" xfId="3" builtinId="30"/>
@@ -362,7 +364,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="108">
+  <dxfs count="36">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -376,802 +378,11 @@
       <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE9FD9F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE593"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCECFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCECFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE9FD9F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE593"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCECFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE9FD9F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE593"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCECFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE9FD9F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE593"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCECFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE9FD9F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE593"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCECFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE9FD9F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE593"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCECFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE9FD9F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE593"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCECFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE9FD9F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE593"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCECFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE9FD9F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE593"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCECFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE9FD9F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE593"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCECFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE9FD9F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE593"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCECFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE9FD9F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE593"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCECFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE9FD9F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE593"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCECFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE9FD9F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE593"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
+      <border outline="0">
+        <top style="thick">
+          <color theme="4" tint="0.499984740745262"/>
+        </top>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1193,10 +404,227 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE593"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE9FD9F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCECFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE593"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE9FD9F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCECFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE593"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE9FD9F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCECFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE593"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE9FD9F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99FF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCECFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99FF99"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <border outline="0">
@@ -1249,41 +677,6 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Gill Sans MT"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
           <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -1299,34 +692,13 @@
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Gill Sans MT"/>
-        <family val="2"/>
-        <scheme val="minor"/>
       </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thick">
-          <color theme="4" tint="0.499984740745262"/>
-        </top>
-      </border>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1543,15 +915,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7787D971-5FA8-482A-8E65-1C7AA4034E42}" name="Table1" displayName="Table1" ref="A11:E25" headerRowDxfId="103" tableBorderDxfId="107">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7787D971-5FA8-482A-8E65-1C7AA4034E42}" name="Table1" displayName="Table1" ref="A11:E25" headerRowDxfId="35" tableBorderDxfId="34">
   <autoFilter ref="A11:E25" xr:uid="{7787D971-5FA8-482A-8E65-1C7AA4034E42}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{01C644CF-7B8F-417A-AA7B-10623F69C84E}" name="Feature is present" totalsRowLabel="Total"/>
     <tableColumn id="2" xr3:uid="{C6E45BFD-6E58-46D8-A1C1-F89BD35A5550}" name="Walking distance to amenity (minutes)"/>
     <tableColumn id="3" xr3:uid="{06DB3AF2-FB10-4AAA-B265-F419AD124469}" name="Feature or Amenity" dataCellStyle="Normal"/>
     <tableColumn id="5" xr3:uid="{24D9BF26-8F1B-4344-9D78-28765136DCA5}" name="Base Score"/>
-    <tableColumn id="4" xr3:uid="{F28DF851-011F-451A-B324-B5BEDE1E5B91}" name="Score" totalsRowFunction="sum" dataDxfId="2" totalsRowDxfId="106" dataCellStyle="20% - Accent1">
-      <calculatedColumnFormula array="1">D12 * _xlfn.IFS(B12&lt;=5,1,B12&lt;=10,0.5,B12&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B12),0) + IF(A12="present",D12,0)</calculatedColumnFormula>
+    <tableColumn id="4" xr3:uid="{F28DF851-011F-451A-B324-B5BEDE1E5B91}" name="Score" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="33" dataCellStyle="20% - Accent1">
+      <calculatedColumnFormula array="1">D12 * _xlfn.IFS(B12&lt;=5,1,B12&lt;=25,(25-B12) / 20, TRUE, 0)*IF(ISBLANK(B12),0,1) + IF(A12="present",D12,0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
@@ -1559,15 +931,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EAB221B2-B100-41A6-952C-DD89F5A01BAE}" name="Table13" displayName="Table13" ref="A29:E49" headerRowDxfId="102" tableBorderDxfId="105">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EAB221B2-B100-41A6-952C-DD89F5A01BAE}" name="Table13" displayName="Table13" ref="A29:E49" headerRowDxfId="4" tableBorderDxfId="3">
   <autoFilter ref="A29:E49" xr:uid="{EAB221B2-B100-41A6-952C-DD89F5A01BAE}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{9A121F8C-AEEA-4E4A-8137-276BD29CFA35}" name="Feature is present" totalsRowLabel="Total"/>
     <tableColumn id="2" xr3:uid="{08DA7BD5-E4BD-46B1-A061-A9DA64DC0AB6}" name="Walking distance to amenity (minutes)"/>
     <tableColumn id="3" xr3:uid="{F381D23A-765B-4D60-A4C6-238AD7D11B59}" name="Feature or Amenity" dataCellStyle="Normal"/>
     <tableColumn id="5" xr3:uid="{90B0D726-BB7E-4845-B6E7-7540996C8AF0}" name="Base Score"/>
-    <tableColumn id="4" xr3:uid="{65F2A830-8A2A-4ACC-A222-34BAEA6782E5}" name="Score" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="104" dataCellStyle="20% - Accent1">
-      <calculatedColumnFormula array="1">D30 * _xlfn.IFS(B30&lt;=5,1,B30&lt;=10,0.5,B30&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B30),0) + IF(A30="present",D30,0)</calculatedColumnFormula>
+    <tableColumn id="4" xr3:uid="{65F2A830-8A2A-4ACC-A222-34BAEA6782E5}" name="Score" totalsRowFunction="sum" dataDxfId="2" dataCellStyle="20% - Accent1">
+      <calculatedColumnFormula array="1">D30 * _xlfn.IFS(B30&lt;=5,1,B30&lt;=25,(25-B30) / 20, TRUE, 0)*IF(ISBLANK(B30),0,1) + IF(A30="present",D30,0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
@@ -1575,15 +947,15 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0BCC82F9-5B3C-44C6-B890-29BBA20B39E0}" name="Table134" displayName="Table134" ref="A53:E61" headerRowDxfId="101" tableBorderDxfId="100">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0BCC82F9-5B3C-44C6-B890-29BBA20B39E0}" name="Table134" displayName="Table134" ref="A53:E61" headerRowDxfId="32" tableBorderDxfId="31">
   <autoFilter ref="A53:E61" xr:uid="{0BCC82F9-5B3C-44C6-B890-29BBA20B39E0}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{04A188A8-03CA-4DF8-82DD-6046CED78BBB}" name="Feature is present" totalsRowLabel="Total"/>
     <tableColumn id="2" xr3:uid="{10335A43-002E-4EBB-B827-076D9CC53921}" name="Walking distance to amenity (minutes)"/>
     <tableColumn id="3" xr3:uid="{B3D3D07A-8652-4629-A378-AD2F7C914601}" name="Feature or Amenity" dataCellStyle="Normal"/>
     <tableColumn id="5" xr3:uid="{39065CE4-0DCD-4C19-80C3-4198D049E444}" name="Base Score"/>
-    <tableColumn id="4" xr3:uid="{6A5035D9-991E-4431-A923-2C3386AC1C0C}" name="Score" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="99" dataCellStyle="20% - Accent1">
-      <calculatedColumnFormula array="1">D54 * _xlfn.IFS(B54&lt;=5,1,B54&lt;=10,0.5,B54&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B54),0) + IF(A54="present",D54,0)</calculatedColumnFormula>
+    <tableColumn id="4" xr3:uid="{6A5035D9-991E-4431-A923-2C3386AC1C0C}" name="Score" totalsRowFunction="sum" dataDxfId="0" dataCellStyle="20% - Accent1">
+      <calculatedColumnFormula array="1">D54 * _xlfn.IFS(B54&lt;=5,1,B54&lt;=25,(25-B54) / 20, TRUE, 0)*IF(ISBLANK(B54),0,1) + IF(A54="present",D54,0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
@@ -1848,7 +1220,7 @@
   <dimension ref="A2:G61"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.35"/>
@@ -1861,67 +1233,70 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="21.75" x14ac:dyDescent="0.45">
-      <c r="F2" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="G2" s="12">
+      <c r="F2" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="10">
         <f>AVERAGE(G3:G5)</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G3" s="13">
+        <v>48</v>
+      </c>
+      <c r="G3" s="11">
         <f>SUM(Table1[Score])/SUM(Table1[Base Score])</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="13">
+        <v>16</v>
+      </c>
+      <c r="G4" s="11">
         <f>SUM(Table13[Score])/SUM(Table13[Base Score])</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" s="13">
+        <v>37</v>
+      </c>
+      <c r="G5" s="11">
         <f>SUM(Table134[Score])/SUM(Table134[Base Score])</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="21" x14ac:dyDescent="0.45">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="5"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="10" t="s">
+      <c r="A11" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="10" t="s">
+      <c r="D11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>52</v>
+      </c>
       <c r="B12" t="s">
         <v>4</v>
       </c>
@@ -1931,8 +1306,8 @@
       <c r="D12">
         <v>3</v>
       </c>
-      <c r="E12" s="7" cm="1">
-        <f t="array" ref="E12">D12 * _xlfn.IFS(B12&lt;=5,1,B12&lt;=10,0.5,B12&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B12),0) + IF(A12="present",D12,0)</f>
+      <c r="E12" s="5" cm="1">
+        <f t="array" ref="E12">D12 * _xlfn.IFS(B12&lt;=5,1,B12&lt;=25,(25-B12) / 20, TRUE, 0)*IF(ISBLANK(B12),0,1) + IF(A12="present",D12,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1946,8 +1321,8 @@
       <c r="D13">
         <v>1</v>
       </c>
-      <c r="E13" s="7" cm="1">
-        <f t="array" ref="E13">D13 * _xlfn.IFS(B13&lt;=5,1,B13&lt;=10,0.5,B13&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B13),0) + IF(A13="present",D13,0)</f>
+      <c r="E13" s="5" cm="1">
+        <f t="array" ref="E13">D13 * _xlfn.IFS(B13&lt;=5,1,B13&lt;=25,(25-B13) / 20, TRUE, 0)*IF(ISBLANK(B13),0,1) + IF(A13="present",D13,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1956,13 +1331,13 @@
         <v>4</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
-      <c r="E14" s="7" cm="1">
-        <f t="array" ref="E14">D14 * _xlfn.IFS(B14&lt;=5,1,B14&lt;=10,0.5,B14&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B14),0) + IF(A14="present",D14,0)</f>
+      <c r="E14" s="5" cm="1">
+        <f t="array" ref="E14">D14 * _xlfn.IFS(B14&lt;=5,1,B14&lt;=25,(25-B14) / 20, TRUE, 0)*IF(ISBLANK(B14),0,1) + IF(A14="present",D14,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1971,13 +1346,13 @@
         <v>4</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
-      <c r="E15" s="7" cm="1">
-        <f t="array" ref="E15">D15 * _xlfn.IFS(B15&lt;=5,1,B15&lt;=10,0.5,B15&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B15),0) + IF(A15="present",D15,0)</f>
+      <c r="E15" s="5" cm="1">
+        <f t="array" ref="E15">D15 * _xlfn.IFS(B15&lt;=5,1,B15&lt;=25,(25-B15) / 20, TRUE, 0)*IF(ISBLANK(B15),0,1) + IF(A15="present",D15,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1986,13 +1361,13 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="D16">
         <v>3</v>
       </c>
-      <c r="E16" s="7" cm="1">
-        <f t="array" ref="E16">D16 * _xlfn.IFS(B16&lt;=5,1,B16&lt;=10,0.5,B16&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B16),0) + IF(A16="present",D16,0)</f>
+      <c r="E16" s="5" cm="1">
+        <f t="array" ref="E16">D16 * _xlfn.IFS(B16&lt;=5,1,B16&lt;=25,(25-B16) / 20, TRUE, 0)*IF(ISBLANK(B16),0,1) + IF(A16="present",D16,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2001,13 +1376,13 @@
         <v>4</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
-      <c r="E17" s="7" cm="1">
-        <f t="array" ref="E17">D17 * _xlfn.IFS(B17&lt;=5,1,B17&lt;=10,0.5,B17&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B17),0) + IF(A17="present",D17,0)</f>
+      <c r="E17" s="5" cm="1">
+        <f t="array" ref="E17">D17 * _xlfn.IFS(B17&lt;=5,1,B17&lt;=25,(25-B17) / 20, TRUE, 0)*IF(ISBLANK(B17),0,1) + IF(A17="present",D17,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2016,13 +1391,13 @@
         <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D18">
         <v>3</v>
       </c>
-      <c r="E18" s="7" cm="1">
-        <f t="array" ref="E18">D18 * _xlfn.IFS(B18&lt;=5,1,B18&lt;=10,0.5,B18&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B18),0) + IF(A18="present",D18,0)</f>
+      <c r="E18" s="5" cm="1">
+        <f t="array" ref="E18">D18 * _xlfn.IFS(B18&lt;=5,1,B18&lt;=25,(25-B18) / 20, TRUE, 0)*IF(ISBLANK(B18),0,1) + IF(A18="present",D18,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2031,13 +1406,13 @@
         <v>4</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D19">
         <v>2</v>
       </c>
-      <c r="E19" s="7" cm="1">
-        <f t="array" ref="E19">D19 * _xlfn.IFS(B19&lt;=5,1,B19&lt;=10,0.5,B19&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B19),0) + IF(A19="present",D19,0)</f>
+      <c r="E19" s="5" cm="1">
+        <f t="array" ref="E19">D19 * _xlfn.IFS(B19&lt;=5,1,B19&lt;=25,(25-B19) / 20, TRUE, 0)*IF(ISBLANK(B19),0,1) + IF(A19="present",D19,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2046,13 +1421,13 @@
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D20">
         <v>2</v>
       </c>
-      <c r="E20" s="7" cm="1">
-        <f t="array" ref="E20">D20 * _xlfn.IFS(B20&lt;=5,1,B20&lt;=10,0.5,B20&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B20),0) + IF(A20="present",D20,0)</f>
+      <c r="E20" s="5" cm="1">
+        <f t="array" ref="E20">D20 * _xlfn.IFS(B20&lt;=5,1,B20&lt;=25,(25-B20) / 20, TRUE, 0)*IF(ISBLANK(B20),0,1) + IF(A20="present",D20,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2061,13 +1436,13 @@
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D21">
         <v>2</v>
       </c>
-      <c r="E21" s="7" cm="1">
-        <f t="array" ref="E21">D21 * _xlfn.IFS(B21&lt;=5,1,B21&lt;=10,0.5,B21&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B21),0) + IF(A21="present",D21,0)</f>
+      <c r="E21" s="5" cm="1">
+        <f t="array" ref="E21">D21 * _xlfn.IFS(B21&lt;=5,1,B21&lt;=25,(25-B21) / 20, TRUE, 0)*IF(ISBLANK(B21),0,1) + IF(A21="present",D21,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2076,13 +1451,13 @@
         <v>4</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
-      <c r="E22" s="7" cm="1">
-        <f t="array" ref="E22">D22 * _xlfn.IFS(B22&lt;=5,1,B22&lt;=10,0.5,B22&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B22),0) + IF(A22="present",D22,0)</f>
+      <c r="E22" s="5" cm="1">
+        <f t="array" ref="E22">D22 * _xlfn.IFS(B22&lt;=5,1,B22&lt;=25,(25-B22) / 20, TRUE, 0)*IF(ISBLANK(B22),0,1) + IF(A22="present",D22,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2091,13 +1466,13 @@
         <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D23">
         <v>2</v>
       </c>
-      <c r="E23" s="8" cm="1">
-        <f t="array" ref="E23">D23 * _xlfn.IFS(B23&lt;=5,1,B23&lt;=10,0.5,B23&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B23),0) + IF(A23="present",D23,0)</f>
+      <c r="E23" s="6" cm="1">
+        <f t="array" ref="E23">D23 * _xlfn.IFS(B23&lt;=5,1,B23&lt;=25,(25-B23) / 20, TRUE, 0)*IF(ISBLANK(B23),0,1) + IF(A23="present",D23,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2105,14 +1480,14 @@
       <c r="B24" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>14</v>
+      <c r="C24" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="D24">
         <v>2</v>
       </c>
-      <c r="E24" s="8" cm="1">
-        <f t="array" ref="E24">D24 * _xlfn.IFS(B24&lt;=5,1,B24&lt;=10,0.5,B24&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B24),0) + IF(A24="present",D24,0)</f>
+      <c r="E24" s="6" cm="1">
+        <f t="array" ref="E24">D24 * _xlfn.IFS(B24&lt;=5,1,B24&lt;=25,(25-B24) / 20, TRUE, 0)*IF(ISBLANK(B24),0,1) + IF(A24="present",D24,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2120,39 +1495,39 @@
       <c r="A25" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="6" t="s">
-        <v>47</v>
+      <c r="C25" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="D25">
         <v>2</v>
       </c>
-      <c r="E25" s="8" cm="1">
-        <f t="array" ref="E25">D25 * _xlfn.IFS(B25&lt;=5,1,B25&lt;=10,0.5,B25&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B25),0) + IF(A25="present",D25,0)</f>
+      <c r="E25" s="6" cm="1">
+        <f t="array" ref="E25">D25 * _xlfn.IFS(B25&lt;=5,1,B25&lt;=25,(25-B25) / 20, TRUE, 0)*IF(ISBLANK(B25),0,1) + IF(A25="present",D25,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="21" x14ac:dyDescent="0.45">
-      <c r="A28" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="5"/>
+      <c r="A28" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="1"/>
     </row>
     <row r="29" spans="1:5" ht="34.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C29" s="10" t="s">
+      <c r="A29" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D29" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="10" t="s">
+      <c r="D29" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2161,13 +1536,13 @@
         <v>4</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D30">
         <v>3</v>
       </c>
-      <c r="E30" s="7" cm="1">
-        <f t="array" ref="E30">D30 * _xlfn.IFS(B30&lt;=5,1,B30&lt;=10,0.5,B30&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B30),0) + IF(A30="present",D30,0)</f>
+      <c r="E30" s="5" cm="1">
+        <f t="array" ref="E30">D30 * _xlfn.IFS(B30&lt;=5,1,B30&lt;=25,(25-B30) / 20, TRUE, 0)*IF(ISBLANK(B30),0,1) + IF(A30="present",D30,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2176,13 +1551,13 @@
         <v>4</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D31">
         <v>3</v>
       </c>
-      <c r="E31" s="7" cm="1">
-        <f t="array" ref="E31">D31 * _xlfn.IFS(B31&lt;=5,1,B31&lt;=10,0.5,B31&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B31),0) + IF(A31="present",D31,0)</f>
+      <c r="E31" s="5" cm="1">
+        <f t="array" ref="E31">D31 * _xlfn.IFS(B31&lt;=5,1,B31&lt;=25,(25-B31) / 20, TRUE, 0)*IF(ISBLANK(B31),0,1) + IF(A31="present",D31,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2191,13 +1566,13 @@
         <v>4</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D32">
         <v>2</v>
       </c>
-      <c r="E32" s="7" cm="1">
-        <f t="array" ref="E32">D32 * _xlfn.IFS(B32&lt;=5,1,B32&lt;=10,0.5,B32&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B32),0) + IF(A32="present",D32,0)</f>
+      <c r="E32" s="5" cm="1">
+        <f t="array" ref="E32">D32 * _xlfn.IFS(B32&lt;=5,1,B32&lt;=25,(25-B32) / 20, TRUE, 0)*IF(ISBLANK(B32),0,1) + IF(A32="present",D32,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2206,13 +1581,13 @@
         <v>4</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D33">
         <v>2</v>
       </c>
-      <c r="E33" s="7" cm="1">
-        <f t="array" ref="E33">D33 * _xlfn.IFS(B33&lt;=5,1,B33&lt;=10,0.5,B33&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B33),0) + IF(A33="present",D33,0)</f>
+      <c r="E33" s="5" cm="1">
+        <f t="array" ref="E33">D33 * _xlfn.IFS(B33&lt;=5,1,B33&lt;=25,(25-B33) / 20, TRUE, 0)*IF(ISBLANK(B33),0,1) + IF(A33="present",D33,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2221,13 +1596,13 @@
         <v>4</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D34">
         <v>2</v>
       </c>
-      <c r="E34" s="7" cm="1">
-        <f t="array" ref="E34">D34 * _xlfn.IFS(B34&lt;=5,1,B34&lt;=10,0.5,B34&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B34),0) + IF(A34="present",D34,0)</f>
+      <c r="E34" s="5" cm="1">
+        <f t="array" ref="E34">D34 * _xlfn.IFS(B34&lt;=5,1,B34&lt;=25,(25-B34) / 20, TRUE, 0)*IF(ISBLANK(B34),0,1) + IF(A34="present",D34,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2236,13 +1611,13 @@
         <v>4</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D35">
         <v>2</v>
       </c>
-      <c r="E35" s="7" cm="1">
-        <f t="array" ref="E35">D35 * _xlfn.IFS(B35&lt;=5,1,B35&lt;=10,0.5,B35&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B35),0) + IF(A35="present",D35,0)</f>
+      <c r="E35" s="5" cm="1">
+        <f t="array" ref="E35">D35 * _xlfn.IFS(B35&lt;=5,1,B35&lt;=25,(25-B35) / 20, TRUE, 0)*IF(ISBLANK(B35),0,1) + IF(A35="present",D35,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2251,13 +1626,13 @@
         <v>4</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D36">
         <v>2</v>
       </c>
-      <c r="E36" s="7" cm="1">
-        <f t="array" ref="E36">D36 * _xlfn.IFS(B36&lt;=5,1,B36&lt;=10,0.5,B36&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B36),0) + IF(A36="present",D36,0)</f>
+      <c r="E36" s="5" cm="1">
+        <f t="array" ref="E36">D36 * _xlfn.IFS(B36&lt;=5,1,B36&lt;=25,(25-B36) / 20, TRUE, 0)*IF(ISBLANK(B36),0,1) + IF(A36="present",D36,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2266,13 +1641,13 @@
         <v>4</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D37">
         <v>2</v>
       </c>
-      <c r="E37" s="7" cm="1">
-        <f t="array" ref="E37">D37 * _xlfn.IFS(B37&lt;=5,1,B37&lt;=10,0.5,B37&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B37),0) + IF(A37="present",D37,0)</f>
+      <c r="E37" s="5" cm="1">
+        <f t="array" ref="E37">D37 * _xlfn.IFS(B37&lt;=5,1,B37&lt;=25,(25-B37) / 20, TRUE, 0)*IF(ISBLANK(B37),0,1) + IF(A37="present",D37,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2281,13 +1656,13 @@
         <v>4</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D38">
         <v>2</v>
       </c>
-      <c r="E38" s="7" cm="1">
-        <f t="array" ref="E38">D38 * _xlfn.IFS(B38&lt;=5,1,B38&lt;=10,0.5,B38&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B38),0) + IF(A38="present",D38,0)</f>
+      <c r="E38" s="5" cm="1">
+        <f t="array" ref="E38">D38 * _xlfn.IFS(B38&lt;=5,1,B38&lt;=25,(25-B38) / 20, TRUE, 0)*IF(ISBLANK(B38),0,1) + IF(A38="present",D38,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2296,13 +1671,13 @@
         <v>4</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D39">
         <v>2</v>
       </c>
-      <c r="E39" s="7" cm="1">
-        <f t="array" ref="E39">D39 * _xlfn.IFS(B39&lt;=5,1,B39&lt;=10,0.5,B39&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B39),0) + IF(A39="present",D39,0)</f>
+      <c r="E39" s="5" cm="1">
+        <f t="array" ref="E39">D39 * _xlfn.IFS(B39&lt;=5,1,B39&lt;=25,(25-B39) / 20, TRUE, 0)*IF(ISBLANK(B39),0,1) + IF(A39="present",D39,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2311,13 +1686,13 @@
         <v>4</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D40">
         <v>2</v>
       </c>
-      <c r="E40" s="7" cm="1">
-        <f t="array" ref="E40">D40 * _xlfn.IFS(B40&lt;=5,1,B40&lt;=10,0.5,B40&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B40),0) + IF(A40="present",D40,0)</f>
+      <c r="E40" s="5" cm="1">
+        <f t="array" ref="E40">D40 * _xlfn.IFS(B40&lt;=5,1,B40&lt;=25,(25-B40) / 20, TRUE, 0)*IF(ISBLANK(B40),0,1) + IF(A40="present",D40,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2326,13 +1701,13 @@
         <v>4</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D41">
         <v>2</v>
       </c>
-      <c r="E41" s="7" cm="1">
-        <f t="array" ref="E41">D41 * _xlfn.IFS(B41&lt;=5,1,B41&lt;=10,0.5,B41&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B41),0) + IF(A41="present",D41,0)</f>
+      <c r="E41" s="5" cm="1">
+        <f t="array" ref="E41">D41 * _xlfn.IFS(B41&lt;=5,1,B41&lt;=25,(25-B41) / 20, TRUE, 0)*IF(ISBLANK(B41),0,1) + IF(A41="present",D41,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2341,13 +1716,13 @@
         <v>4</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D42">
         <v>2</v>
       </c>
-      <c r="E42" s="7" cm="1">
-        <f t="array" ref="E42">D42 * _xlfn.IFS(B42&lt;=5,1,B42&lt;=10,0.5,B42&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B42),0) + IF(A42="present",D42,0)</f>
+      <c r="E42" s="5" cm="1">
+        <f t="array" ref="E42">D42 * _xlfn.IFS(B42&lt;=5,1,B42&lt;=25,(25-B42) / 20, TRUE, 0)*IF(ISBLANK(B42),0,1) + IF(A42="present",D42,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2356,13 +1731,13 @@
         <v>4</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D43">
         <v>2</v>
       </c>
-      <c r="E43" s="7" cm="1">
-        <f t="array" ref="E43">D43 * _xlfn.IFS(B43&lt;=5,1,B43&lt;=10,0.5,B43&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B43),0) + IF(A43="present",D43,0)</f>
+      <c r="E43" s="5" cm="1">
+        <f t="array" ref="E43">D43 * _xlfn.IFS(B43&lt;=5,1,B43&lt;=25,(25-B43) / 20, TRUE, 0)*IF(ISBLANK(B43),0,1) + IF(A43="present",D43,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2371,13 +1746,13 @@
         <v>4</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D44">
         <v>2</v>
       </c>
-      <c r="E44" s="7" cm="1">
-        <f t="array" ref="E44">D44 * _xlfn.IFS(B44&lt;=5,1,B44&lt;=10,0.5,B44&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B44),0) + IF(A44="present",D44,0)</f>
+      <c r="E44" s="5" cm="1">
+        <f t="array" ref="E44">D44 * _xlfn.IFS(B44&lt;=5,1,B44&lt;=25,(25-B44) / 20, TRUE, 0)*IF(ISBLANK(B44),0,1) + IF(A44="present",D44,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2386,13 +1761,13 @@
         <v>4</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D45">
         <v>1</v>
       </c>
-      <c r="E45" s="7" cm="1">
-        <f t="array" ref="E45">D45 * _xlfn.IFS(B45&lt;=5,1,B45&lt;=10,0.5,B45&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B45),0) + IF(A45="present",D45,0)</f>
+      <c r="E45" s="5" cm="1">
+        <f t="array" ref="E45">D45 * _xlfn.IFS(B45&lt;=5,1,B45&lt;=25,(25-B45) / 20, TRUE, 0)*IF(ISBLANK(B45),0,1) + IF(A45="present",D45,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2401,13 +1776,13 @@
         <v>4</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D46">
         <v>1</v>
       </c>
-      <c r="E46" s="7" cm="1">
-        <f t="array" ref="E46">D46 * _xlfn.IFS(B46&lt;=5,1,B46&lt;=10,0.5,B46&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B46),0) + IF(A46="present",D46,0)</f>
+      <c r="E46" s="5" cm="1">
+        <f t="array" ref="E46">D46 * _xlfn.IFS(B46&lt;=5,1,B46&lt;=25,(25-B46) / 20, TRUE, 0)*IF(ISBLANK(B46),0,1) + IF(A46="present",D46,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2416,13 +1791,13 @@
         <v>4</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D47">
         <v>1</v>
       </c>
-      <c r="E47" s="7" cm="1">
-        <f t="array" ref="E47">D47 * _xlfn.IFS(B47&lt;=5,1,B47&lt;=10,0.5,B47&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B47),0) + IF(A47="present",D47,0)</f>
+      <c r="E47" s="5" cm="1">
+        <f t="array" ref="E47">D47 * _xlfn.IFS(B47&lt;=5,1,B47&lt;=25,(25-B47) / 20, TRUE, 0)*IF(ISBLANK(B47),0,1) + IF(A47="present",D47,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2431,13 +1806,13 @@
         <v>4</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D48">
         <v>1</v>
       </c>
-      <c r="E48" s="7" cm="1">
-        <f t="array" ref="E48">D48 * _xlfn.IFS(B48&lt;=5,1,B48&lt;=10,0.5,B48&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B48),0) + IF(A48="present",D48,0)</f>
+      <c r="E48" s="5" cm="1">
+        <f t="array" ref="E48">D48 * _xlfn.IFS(B48&lt;=5,1,B48&lt;=25,(25-B48) / 20, TRUE, 0)*IF(ISBLANK(B48),0,1) + IF(A48="present",D48,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2446,38 +1821,38 @@
         <v>4</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D49">
         <v>1</v>
       </c>
-      <c r="E49" s="7" cm="1">
-        <f t="array" ref="E49">D49 * _xlfn.IFS(B49&lt;=5,1,B49&lt;=10,0.5,B49&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B49),0) + IF(A49="present",D49,0)</f>
+      <c r="E49" s="5" cm="1">
+        <f t="array" ref="E49">D49 * _xlfn.IFS(B49&lt;=5,1,B49&lt;=25,(25-B49) / 20, TRUE, 0)*IF(ISBLANK(B49),0,1) + IF(A49="present",D49,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="21" x14ac:dyDescent="0.45">
-      <c r="A52" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="5"/>
+      <c r="A52" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B52" s="12"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="1"/>
     </row>
     <row r="53" spans="1:5" ht="34.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B53" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C53" s="10" t="s">
+      <c r="A53" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C53" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D53" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E53" s="10" t="s">
+      <c r="D53" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2486,13 +1861,13 @@
         <v>4</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D54">
         <v>3</v>
       </c>
-      <c r="E54" s="7" cm="1">
-        <f t="array" ref="E54">D54 * _xlfn.IFS(B54&lt;=5,1,B54&lt;=10,0.5,B54&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B54),0) + IF(A54="present",D54,0)</f>
+      <c r="E54" s="5" cm="1">
+        <f t="array" ref="E54">D54 * _xlfn.IFS(B54&lt;=5,1,B54&lt;=25,(25-B54) / 20, TRUE, 0)*IF(ISBLANK(B54),0,1) + IF(A54="present",D54,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2501,13 +1876,13 @@
         <v>4</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D55">
         <v>3</v>
       </c>
-      <c r="E55" s="7" cm="1">
-        <f t="array" ref="E55">D55 * _xlfn.IFS(B55&lt;=5,1,B55&lt;=10,0.5,B55&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B55),0) + IF(A55="present",D55,0)</f>
+      <c r="E55" s="5" cm="1">
+        <f t="array" ref="E55">D55 * _xlfn.IFS(B55&lt;=5,1,B55&lt;=25,(25-B55) / 20, TRUE, 0)*IF(ISBLANK(B55),0,1) + IF(A55="present",D55,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2516,13 +1891,13 @@
         <v>4</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D56">
         <v>2</v>
       </c>
-      <c r="E56" s="7" cm="1">
-        <f t="array" ref="E56">D56 * _xlfn.IFS(B56&lt;=5,1,B56&lt;=10,0.5,B56&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B56),0) + IF(A56="present",D56,0)</f>
+      <c r="E56" s="5" cm="1">
+        <f t="array" ref="E56">D56 * _xlfn.IFS(B56&lt;=5,1,B56&lt;=25,(25-B56) / 20, TRUE, 0)*IF(ISBLANK(B56),0,1) + IF(A56="present",D56,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2531,13 +1906,13 @@
         <v>4</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D57">
         <v>2</v>
       </c>
-      <c r="E57" s="7" cm="1">
-        <f t="array" ref="E57">D57 * _xlfn.IFS(B57&lt;=5,1,B57&lt;=10,0.5,B57&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B57),0) + IF(A57="present",D57,0)</f>
+      <c r="E57" s="5" cm="1">
+        <f t="array" ref="E57">D57 * _xlfn.IFS(B57&lt;=5,1,B57&lt;=25,(25-B57) / 20, TRUE, 0)*IF(ISBLANK(B57),0,1) + IF(A57="present",D57,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2546,13 +1921,13 @@
         <v>4</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D58">
         <v>1</v>
       </c>
-      <c r="E58" s="7" cm="1">
-        <f t="array" ref="E58">D58 * _xlfn.IFS(B58&lt;=5,1,B58&lt;=10,0.5,B58&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B58),0) + IF(A58="present",D58,0)</f>
+      <c r="E58" s="5" cm="1">
+        <f t="array" ref="E58">D58 * _xlfn.IFS(B58&lt;=5,1,B58&lt;=25,(25-B58) / 20, TRUE, 0)*IF(ISBLANK(B58),0,1) + IF(A58="present",D58,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2561,13 +1936,13 @@
         <v>4</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D59">
         <v>1</v>
       </c>
-      <c r="E59" s="7" cm="1">
-        <f t="array" ref="E59">D59 * _xlfn.IFS(B59&lt;=5,1,B59&lt;=10,0.5,B59&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B59),0) + IF(A59="present",D59,0)</f>
+      <c r="E59" s="5" cm="1">
+        <f t="array" ref="E59">D59 * _xlfn.IFS(B59&lt;=5,1,B59&lt;=25,(25-B59) / 20, TRUE, 0)*IF(ISBLANK(B59),0,1) + IF(A59="present",D59,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2576,13 +1951,13 @@
         <v>4</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D60">
         <v>1</v>
       </c>
-      <c r="E60" s="7" cm="1">
-        <f t="array" ref="E60">D60 * _xlfn.IFS(B60&lt;=5,1,B60&lt;=10,0.5,B60&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B60),0) + IF(A60="present",D60,0)</f>
+      <c r="E60" s="5" cm="1">
+        <f t="array" ref="E60">D60 * _xlfn.IFS(B60&lt;=5,1,B60&lt;=25,(25-B60) / 20, TRUE, 0)*IF(ISBLANK(B60),0,1) + IF(A60="present",D60,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2591,13 +1966,13 @@
         <v>4</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D61">
         <v>1</v>
       </c>
-      <c r="E61" s="7" cm="1">
-        <f t="array" ref="E61">D61 * _xlfn.IFS(B61&lt;=5,1,B61&lt;=10,0.5,B61&lt;=20,0.25,TRUE,0)*IF(ISBLANK(B61),0) + IF(A61="present",D61,0)</f>
+      <c r="E61" s="5" cm="1">
+        <f t="array" ref="E61">D61 * _xlfn.IFS(B61&lt;=5,1,B61&lt;=25,(25-B61) / 20, TRUE, 0)*IF(ISBLANK(B61),0,1) + IF(A61="present",D61,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2608,100 +1983,100 @@
     <mergeCell ref="A52:C52"/>
   </mergeCells>
   <conditionalFormatting sqref="A12:A17 A19:A25">
-    <cfRule type="cellIs" dxfId="50" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="39" operator="equal">
       <formula>"present"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A30:A49">
+    <cfRule type="cellIs" dxfId="29" priority="4" operator="equal">
+      <formula>"N/A"</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="28" priority="5">
+      <formula>LEN(TRIM(A30))=0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="6" operator="equal">
+      <formula>"absent"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A54:A61">
+    <cfRule type="cellIs" dxfId="26" priority="13" operator="equal">
+      <formula>"present"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A56">
+    <cfRule type="cellIs" dxfId="25" priority="1" operator="lessThanOrEqual">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="lessThanOrEqual">
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="3" operator="lessThanOrEqual">
+      <formula>20</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12:B25 B44:B49">
+    <cfRule type="cellIs" dxfId="22" priority="32" operator="equal">
+      <formula>"absent"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A54:B61">
+    <cfRule type="cellIs" dxfId="21" priority="7" operator="equal">
+      <formula>"N/A"</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="20" priority="8">
+      <formula>LEN(TRIM(A54))=0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="12" operator="equal">
+      <formula>"absent"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B25 B44:B49">
-    <cfRule type="cellIs" dxfId="49" priority="31" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="18" priority="29" operator="lessThanOrEqual">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="30" operator="lessThanOrEqual">
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="31" operator="lessThanOrEqual">
       <formula>20</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="30" operator="lessThanOrEqual">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B30:B49">
+    <cfRule type="cellIs" dxfId="15" priority="20" operator="equal">
+      <formula>"N/A"</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="14" priority="21">
+      <formula>LEN(TRIM(B30))=0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="22" operator="lessThanOrEqual">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="23" operator="lessThanOrEqual">
       <formula>10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="29" operator="lessThanOrEqual">
-      <formula>5</formula>
+    <cfRule type="cellIs" dxfId="11" priority="24" operator="lessThanOrEqual">
+      <formula>20</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="25" operator="equal">
+      <formula>"absent"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44:B49 A12:B25">
-    <cfRule type="cellIs" dxfId="46" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="27" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="45" priority="28">
+    <cfRule type="containsBlanks" dxfId="8" priority="28">
       <formula>LEN(TRIM(A12))=0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="32" operator="equal">
-      <formula>"absent"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B30:B49">
-    <cfRule type="cellIs" dxfId="42" priority="24" operator="lessThanOrEqual">
-      <formula>20</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="23" operator="lessThanOrEqual">
-      <formula>10</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="22" operator="lessThanOrEqual">
-      <formula>5</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B30:B49">
-    <cfRule type="cellIs" dxfId="39" priority="20" operator="equal">
-      <formula>"N/A"</formula>
-    </cfRule>
-    <cfRule type="containsBlanks" dxfId="38" priority="21">
-      <formula>LEN(TRIM(B30))=0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="25" operator="equal">
-      <formula>"absent"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A54:A61">
-    <cfRule type="cellIs" dxfId="36" priority="13" operator="equal">
-      <formula>"present"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B54:B61">
-    <cfRule type="cellIs" dxfId="35" priority="11" operator="lessThanOrEqual">
-      <formula>20</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="10" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="lessThanOrEqual">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="10" operator="lessThanOrEqual">
       <formula>10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="9" operator="lessThanOrEqual">
-      <formula>5</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A54:B61">
-    <cfRule type="cellIs" dxfId="32" priority="7" operator="equal">
-      <formula>"N/A"</formula>
-    </cfRule>
-    <cfRule type="containsBlanks" dxfId="31" priority="8">
-      <formula>LEN(TRIM(A54))=0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="12" operator="equal">
-      <formula>"absent"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A30:A49">
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
-      <formula>"N/A"</formula>
-    </cfRule>
-    <cfRule type="containsBlanks" dxfId="7" priority="5">
-      <formula>LEN(TRIM(A30))=0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
-      <formula>"absent"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A56">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThanOrEqual">
-      <formula>5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThanOrEqual">
-      <formula>10</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="5" priority="11" operator="lessThanOrEqual">
       <formula>20</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>